<commit_message>
Updates to diagrams + agile development
</commit_message>
<xml_diff>
--- a/ProcessDocumentation/work-in-progress/workflow-diagrams.xlsx
+++ b/ProcessDocumentation/work-in-progress/workflow-diagrams.xlsx
@@ -4,25 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Project Stage Gates" sheetId="1" r:id="rId1"/>
     <sheet name="SCRUM WorkFlow" sheetId="2" r:id="rId2"/>
-    <sheet name="Life of a bug" sheetId="3" r:id="rId3"/>
+    <sheet name="Development Environment" sheetId="3" r:id="rId3"/>
     <sheet name="Life of a risk" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -32,6 +28,21 @@
     </font>
     <font>
       <sz val="28"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -58,12 +69,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5646,6 +5661,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{10E62C64-2565-44E0-A187-2F2B10393178}" type="pres">
       <dgm:prSet presAssocID="{EA65BA12-EB14-4B0C-9B75-BC6108B5E6EC}" presName="composite" presStyleCnt="0"/>
@@ -5660,10 +5682,24 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{AFDCFD64-1E34-46F0-9AAA-AC6E69919F59}" type="pres">
       <dgm:prSet presAssocID="{EA65BA12-EB14-4B0C-9B75-BC6108B5E6EC}" presName="parSh" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{CE3F3A45-904A-4036-BF2D-3EA3E66AA755}" type="pres">
       <dgm:prSet presAssocID="{EA65BA12-EB14-4B0C-9B75-BC6108B5E6EC}" presName="desTx" presStyleLbl="fgAcc1" presStyleIdx="0" presStyleCnt="4">
@@ -5683,10 +5719,24 @@
     <dgm:pt modelId="{5E6A2DC5-56B0-4E09-B591-2EAD6C544736}" type="pres">
       <dgm:prSet presAssocID="{A9295B5A-7E85-4136-8399-A9D1093354C9}" presName="sibTrans" presStyleLbl="sibTrans2D1" presStyleIdx="0" presStyleCnt="3"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{A1EB640A-C53F-4433-B19E-A29F12213510}" type="pres">
       <dgm:prSet presAssocID="{A9295B5A-7E85-4136-8399-A9D1093354C9}" presName="connTx" presStyleLbl="sibTrans2D1" presStyleIdx="0" presStyleCnt="3"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{CF19F201-2A18-4285-A8E1-57A4CE9D8A37}" type="pres">
       <dgm:prSet presAssocID="{80B88FB7-2385-4524-BD05-D76123E43C84}" presName="composite" presStyleCnt="0"/>
@@ -5701,10 +5751,24 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{A126F55F-5E5E-4048-A1F1-977B4080077A}" type="pres">
       <dgm:prSet presAssocID="{80B88FB7-2385-4524-BD05-D76123E43C84}" presName="parSh" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{4C7B5616-120F-449F-ABFF-689082DA022A}" type="pres">
       <dgm:prSet presAssocID="{80B88FB7-2385-4524-BD05-D76123E43C84}" presName="desTx" presStyleLbl="fgAcc1" presStyleIdx="1" presStyleCnt="4">
@@ -5724,10 +5788,24 @@
     <dgm:pt modelId="{24FF65C9-B0A6-443D-99DA-DD2FC56B4567}" type="pres">
       <dgm:prSet presAssocID="{0433CD39-2D45-456A-A753-06841BB2DB61}" presName="sibTrans" presStyleLbl="sibTrans2D1" presStyleIdx="1" presStyleCnt="3"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{75A349A9-095A-4122-A73F-9F88EF394C0F}" type="pres">
       <dgm:prSet presAssocID="{0433CD39-2D45-456A-A753-06841BB2DB61}" presName="connTx" presStyleLbl="sibTrans2D1" presStyleIdx="1" presStyleCnt="3"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{E6131EB3-2DDF-4FD2-A2D9-AE58DB730A99}" type="pres">
       <dgm:prSet presAssocID="{AEEDE706-77F4-46CD-999E-839BF57EFA0B}" presName="composite" presStyleCnt="0"/>
@@ -5742,10 +5820,24 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{9A4408C1-581B-45E5-B477-B81D20AD7F26}" type="pres">
       <dgm:prSet presAssocID="{AEEDE706-77F4-46CD-999E-839BF57EFA0B}" presName="parSh" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{4B8C0D95-5716-45B7-A556-C54E19DAD819}" type="pres">
       <dgm:prSet presAssocID="{AEEDE706-77F4-46CD-999E-839BF57EFA0B}" presName="desTx" presStyleLbl="fgAcc1" presStyleIdx="2" presStyleCnt="4">
@@ -5765,10 +5857,24 @@
     <dgm:pt modelId="{3ECB40F0-820C-46E0-A0CD-E724EF03AB7D}" type="pres">
       <dgm:prSet presAssocID="{6729120F-A470-4527-BF11-A7AD53B0DE69}" presName="sibTrans" presStyleLbl="sibTrans2D1" presStyleIdx="2" presStyleCnt="3"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{43522153-80A9-444F-8A86-9ECDE283910C}" type="pres">
       <dgm:prSet presAssocID="{6729120F-A470-4527-BF11-A7AD53B0DE69}" presName="connTx" presStyleLbl="sibTrans2D1" presStyleIdx="2" presStyleCnt="3"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{2FB65F33-0EFF-4FC1-A4F5-B484664BB2EE}" type="pres">
       <dgm:prSet presAssocID="{09F81B39-8EE5-4072-94CE-C8399C47BB0C}" presName="composite" presStyleCnt="0"/>
@@ -5783,10 +5889,24 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{CA1357E0-AE94-4CE2-A445-2167652802D8}" type="pres">
       <dgm:prSet presAssocID="{09F81B39-8EE5-4072-94CE-C8399C47BB0C}" presName="parSh" presStyleLbl="node1" presStyleIdx="3" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{9B6422CC-2491-4CA6-8D72-9D9C1E97A8DD}" type="pres">
       <dgm:prSet presAssocID="{09F81B39-8EE5-4072-94CE-C8399C47BB0C}" presName="desTx" presStyleLbl="fgAcc1" presStyleIdx="3" presStyleCnt="4">
@@ -5810,11 +5930,11 @@
     <dgm:cxn modelId="{F0749991-1771-4D87-8810-DA9C77D6F5FA}" type="presOf" srcId="{6729120F-A470-4527-BF11-A7AD53B0DE69}" destId="{3ECB40F0-820C-46E0-A0CD-E724EF03AB7D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
     <dgm:cxn modelId="{D05C566F-3566-4F9A-BF37-E3ED3003B2B2}" type="presOf" srcId="{0433CD39-2D45-456A-A753-06841BB2DB61}" destId="{24FF65C9-B0A6-443D-99DA-DD2FC56B4567}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
     <dgm:cxn modelId="{2012B86A-9CD3-488A-B831-4180105C34DB}" type="presOf" srcId="{EA65BA12-EB14-4B0C-9B75-BC6108B5E6EC}" destId="{22349AE9-A4FB-4060-99AD-EA8097A08EEC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
+    <dgm:cxn modelId="{8CE7742E-45FF-4CE5-8258-26A163397280}" type="presOf" srcId="{6729120F-A470-4527-BF11-A7AD53B0DE69}" destId="{43522153-80A9-444F-8A86-9ECDE283910C}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
     <dgm:cxn modelId="{5CC6333C-DA00-4F7B-AD46-36A935362CD9}" type="presOf" srcId="{80B88FB7-2385-4524-BD05-D76123E43C84}" destId="{309725C4-55DE-4DAD-AD24-836F07B708B4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
-    <dgm:cxn modelId="{8CE7742E-45FF-4CE5-8258-26A163397280}" type="presOf" srcId="{6729120F-A470-4527-BF11-A7AD53B0DE69}" destId="{43522153-80A9-444F-8A86-9ECDE283910C}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
     <dgm:cxn modelId="{AAB7DED0-D3B5-44E3-801F-27BCE93B4C45}" type="presOf" srcId="{80B88FB7-2385-4524-BD05-D76123E43C84}" destId="{A126F55F-5E5E-4048-A1F1-977B4080077A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
+    <dgm:cxn modelId="{B6DB02EB-CF2D-4CD4-A02C-69576DC4F0F7}" srcId="{EA65BA12-EB14-4B0C-9B75-BC6108B5E6EC}" destId="{0A8D4ABC-757C-4B43-804E-722990077524}" srcOrd="0" destOrd="0" parTransId="{65E1AFD4-3901-40D0-9743-F4009F6A7CE3}" sibTransId="{D21FB909-1537-4A44-9C3F-75A052E2CE4B}"/>
     <dgm:cxn modelId="{67C00F1D-6A67-449E-9F8E-6C1B3F8E1C35}" type="presOf" srcId="{FB19170B-360B-4654-88DD-79C33FF24295}" destId="{28672188-53BB-4629-AD01-CBB451947323}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
-    <dgm:cxn modelId="{B6DB02EB-CF2D-4CD4-A02C-69576DC4F0F7}" srcId="{EA65BA12-EB14-4B0C-9B75-BC6108B5E6EC}" destId="{0A8D4ABC-757C-4B43-804E-722990077524}" srcOrd="0" destOrd="0" parTransId="{65E1AFD4-3901-40D0-9743-F4009F6A7CE3}" sibTransId="{D21FB909-1537-4A44-9C3F-75A052E2CE4B}"/>
     <dgm:cxn modelId="{BA4331BF-3516-40C9-AF42-7BF4D5F75FE7}" type="presOf" srcId="{57727E90-DB1C-455C-A0DA-E377135379A6}" destId="{4C7B5616-120F-449F-ABFF-689082DA022A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
     <dgm:cxn modelId="{7E99747B-8F45-4BA7-8E36-1D755E5D066C}" srcId="{FB19170B-360B-4654-88DD-79C33FF24295}" destId="{09F81B39-8EE5-4072-94CE-C8399C47BB0C}" srcOrd="3" destOrd="0" parTransId="{8D83E5B8-9681-4A00-9E21-AC5F1641A5F1}" sibTransId="{F0EF61C1-71D6-49E1-8BE2-858E1AAB5F83}"/>
     <dgm:cxn modelId="{C96B3994-24C9-4EF7-8507-FA60EF8690CC}" type="presOf" srcId="{FD1EE22E-38B9-4196-A07A-3E0E01DEAE8A}" destId="{4B8C0D95-5716-45B7-A556-C54E19DAD819}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
@@ -5825,8 +5945,8 @@
     <dgm:cxn modelId="{5B90FCED-5F6B-4456-8DBB-8D3DEAEC02B5}" type="presOf" srcId="{0A8D4ABC-757C-4B43-804E-722990077524}" destId="{CE3F3A45-904A-4036-BF2D-3EA3E66AA755}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
     <dgm:cxn modelId="{10879DA2-6511-4AD3-86E6-08FCE69AD08A}" srcId="{FB19170B-360B-4654-88DD-79C33FF24295}" destId="{EA65BA12-EB14-4B0C-9B75-BC6108B5E6EC}" srcOrd="0" destOrd="0" parTransId="{97E310D9-60FD-4F77-9246-B1911DB0F736}" sibTransId="{A9295B5A-7E85-4136-8399-A9D1093354C9}"/>
     <dgm:cxn modelId="{C79CC54C-827A-48F6-BBCF-AA9E65A1FDA9}" type="presOf" srcId="{AEEDE706-77F4-46CD-999E-839BF57EFA0B}" destId="{72AA7C93-0DA4-4BC6-B512-9061DAA0CD30}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
+    <dgm:cxn modelId="{93599912-B3F3-4D45-BE29-F4715BA46895}" srcId="{09F81B39-8EE5-4072-94CE-C8399C47BB0C}" destId="{6623748A-FCAF-41A1-81AD-FCC5CDD7A4BC}" srcOrd="0" destOrd="0" parTransId="{E45E3AE3-6749-4123-9BC4-C230658ADEE1}" sibTransId="{B62CDF93-05DF-4AC0-A1CF-4F596309171C}"/>
     <dgm:cxn modelId="{33412374-2FB3-4E2D-8BBF-DF2CB326830D}" srcId="{FB19170B-360B-4654-88DD-79C33FF24295}" destId="{AEEDE706-77F4-46CD-999E-839BF57EFA0B}" srcOrd="2" destOrd="0" parTransId="{C9B29839-B53D-43B9-96D5-FF95A9D12E8C}" sibTransId="{6729120F-A470-4527-BF11-A7AD53B0DE69}"/>
-    <dgm:cxn modelId="{93599912-B3F3-4D45-BE29-F4715BA46895}" srcId="{09F81B39-8EE5-4072-94CE-C8399C47BB0C}" destId="{6623748A-FCAF-41A1-81AD-FCC5CDD7A4BC}" srcOrd="0" destOrd="0" parTransId="{E45E3AE3-6749-4123-9BC4-C230658ADEE1}" sibTransId="{B62CDF93-05DF-4AC0-A1CF-4F596309171C}"/>
     <dgm:cxn modelId="{6F7DE620-949E-4489-AD2D-1BF3E30229B0}" type="presOf" srcId="{09F81B39-8EE5-4072-94CE-C8399C47BB0C}" destId="{CA1357E0-AE94-4CE2-A445-2167652802D8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
     <dgm:cxn modelId="{32DD41A8-7DC8-4755-B4FF-BB0BA49F3568}" type="presOf" srcId="{09F81B39-8EE5-4072-94CE-C8399C47BB0C}" destId="{454BF75C-A4A8-4457-BF0C-00D31990196B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process3"/>
     <dgm:cxn modelId="{D12C5D02-F3A4-4C35-9724-FE97D3EEFFAE}" srcId="{AEEDE706-77F4-46CD-999E-839BF57EFA0B}" destId="{FD1EE22E-38B9-4196-A07A-3E0E01DEAE8A}" srcOrd="0" destOrd="0" parTransId="{2DA1910C-5330-4D71-8BB9-8BAEB09240E2}" sibTransId="{7230A550-B7FF-46EA-B98E-BEB903B0F7F0}"/>
@@ -5939,23 +6059,44 @@
     <dgm:pt modelId="{20929601-342C-4386-8A91-B3B3783D4312}" type="pres">
       <dgm:prSet presAssocID="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" presName="gear1srcNode" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{26EEF785-7D27-4D22-AA6C-A9EF7259F5C0}" type="pres">
       <dgm:prSet presAssocID="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" presName="gear1dstNode" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{55668FCA-7151-45C4-9C4A-50CBC9867591}" type="pres">
       <dgm:prSet presAssocID="{35436CF1-1F89-487D-84AB-6E5616D66864}" presName="connector1" presStyleLbl="sibTrans2D1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
-    <dgm:cxn modelId="{DC5267BA-B565-4C78-92D1-5D65E3C42D02}" type="presOf" srcId="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" destId="{9D63658B-5B03-4CDC-B06D-A3802A94462A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/gear1"/>
-    <dgm:cxn modelId="{697B0035-E63B-444E-8BCF-F6D1C6B58670}" type="presOf" srcId="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" destId="{26EEF785-7D27-4D22-AA6C-A9EF7259F5C0}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/gear1"/>
+    <dgm:cxn modelId="{58AEC938-7C6E-4F38-B64E-19B851EFADEE}" type="presOf" srcId="{35436CF1-1F89-487D-84AB-6E5616D66864}" destId="{55668FCA-7151-45C4-9C4A-50CBC9867591}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/gear1"/>
     <dgm:cxn modelId="{7C4DDC26-14A8-4B0F-86F6-4D49B55133C8}" type="presOf" srcId="{ABA6D5A4-96F4-4394-AE2B-F48CD7295922}" destId="{0CCC68E4-45FC-4735-9D20-7CCBE029E99F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/gear1"/>
     <dgm:cxn modelId="{918D7B59-EFAA-486A-89F1-4DA3A21E4184}" type="presOf" srcId="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" destId="{20929601-342C-4386-8A91-B3B3783D4312}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/gear1"/>
     <dgm:cxn modelId="{312CE1A8-4C8F-47E8-9127-4B063F32B67A}" srcId="{ABA6D5A4-96F4-4394-AE2B-F48CD7295922}" destId="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" srcOrd="0" destOrd="0" parTransId="{41EBF33A-1CB7-44B3-A5A4-EFD51BDA3122}" sibTransId="{35436CF1-1F89-487D-84AB-6E5616D66864}"/>
-    <dgm:cxn modelId="{58AEC938-7C6E-4F38-B64E-19B851EFADEE}" type="presOf" srcId="{35436CF1-1F89-487D-84AB-6E5616D66864}" destId="{55668FCA-7151-45C4-9C4A-50CBC9867591}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/gear1"/>
+    <dgm:cxn modelId="{697B0035-E63B-444E-8BCF-F6D1C6B58670}" type="presOf" srcId="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" destId="{26EEF785-7D27-4D22-AA6C-A9EF7259F5C0}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/gear1"/>
+    <dgm:cxn modelId="{DC5267BA-B565-4C78-92D1-5D65E3C42D02}" type="presOf" srcId="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" destId="{9D63658B-5B03-4CDC-B06D-A3802A94462A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/gear1"/>
     <dgm:cxn modelId="{172EB562-1164-41CE-AD68-7BFC750B8FDB}" type="presParOf" srcId="{0CCC68E4-45FC-4735-9D20-7CCBE029E99F}" destId="{9D63658B-5B03-4CDC-B06D-A3802A94462A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/gear1"/>
     <dgm:cxn modelId="{5D6A3A8E-82F5-4505-A068-16269E048083}" type="presParOf" srcId="{0CCC68E4-45FC-4735-9D20-7CCBE029E99F}" destId="{20929601-342C-4386-8A91-B3B3783D4312}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/gear1"/>
     <dgm:cxn modelId="{91C39F69-678E-476C-A594-D0A4A091E9DE}" type="presParOf" srcId="{0CCC68E4-45FC-4735-9D20-7CCBE029E99F}" destId="{26EEF785-7D27-4D22-AA6C-A9EF7259F5C0}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/gear1"/>
@@ -6043,14 +6184,35 @@
     <dgm:pt modelId="{20929601-342C-4386-8A91-B3B3783D4312}" type="pres">
       <dgm:prSet presAssocID="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" presName="gear1srcNode" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{26EEF785-7D27-4D22-AA6C-A9EF7259F5C0}" type="pres">
       <dgm:prSet presAssocID="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" presName="gear1dstNode" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{55668FCA-7151-45C4-9C4A-50CBC9867591}" type="pres">
       <dgm:prSet presAssocID="{35436CF1-1F89-487D-84AB-6E5616D66864}" presName="connector1" presStyleLbl="sibTrans2D1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
@@ -6147,14 +6309,35 @@
     <dgm:pt modelId="{20929601-342C-4386-8A91-B3B3783D4312}" type="pres">
       <dgm:prSet presAssocID="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" presName="gear1srcNode" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{26EEF785-7D27-4D22-AA6C-A9EF7259F5C0}" type="pres">
       <dgm:prSet presAssocID="{6DA595BB-0A59-48F8-98B0-2DDAA5164F8E}" presName="gear1dstNode" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{55668FCA-7151-45C4-9C4A-50CBC9867591}" type="pres">
       <dgm:prSet presAssocID="{35436CF1-1F89-487D-84AB-6E5616D66864}" presName="connector1" presStyleLbl="sibTrans2D1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
@@ -6195,7 +6378,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB"/>
-            <a:t>Ready</a:t>
+            <a:t>In Progress</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -6231,7 +6414,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB"/>
-            <a:t>In Progress</a:t>
+            <a:t>In Review</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -6321,10 +6504,24 @@
     <dgm:pt modelId="{723000EF-22DF-4167-B710-9FF66AE068F7}" type="pres">
       <dgm:prSet presAssocID="{23F2D4E7-8956-4156-B653-43BFFD3E8868}" presName="sibTrans" presStyleLbl="sibTrans2D1" presStyleIdx="0" presStyleCnt="2"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{A3694BF4-9E7E-4105-96F1-11491276EA6A}" type="pres">
       <dgm:prSet presAssocID="{23F2D4E7-8956-4156-B653-43BFFD3E8868}" presName="connectorText" presStyleLbl="sibTrans2D1" presStyleIdx="0" presStyleCnt="2"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{F2C593C8-199E-4BE8-A2F4-C6746DA80C23}" type="pres">
       <dgm:prSet presAssocID="{A01F4A42-1918-4A19-8090-8A089D6BD25A}" presName="node" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="3">
@@ -6344,10 +6541,24 @@
     <dgm:pt modelId="{F0DF1363-D6A2-49C2-A60C-3630AFB61E67}" type="pres">
       <dgm:prSet presAssocID="{3F994207-2612-453E-A085-A37710E7F755}" presName="sibTrans" presStyleLbl="sibTrans2D1" presStyleIdx="1" presStyleCnt="2"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{3C669D7C-9D20-4333-8B9B-7AF4764D3499}" type="pres">
       <dgm:prSet presAssocID="{3F994207-2612-453E-A085-A37710E7F755}" presName="connectorText" presStyleLbl="sibTrans2D1" presStyleIdx="1" presStyleCnt="2"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{EE8F5E6F-4C60-4DAA-94DE-61E5FFCF9287}" type="pres">
       <dgm:prSet presAssocID="{D1F4FBF3-0DDB-4943-9E2C-1C88BE4D0831}" presName="node" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="3">
@@ -6371,8 +6582,8 @@
     <dgm:cxn modelId="{DBC19182-F854-4AD3-9C04-59EC5D9DD77D}" type="presOf" srcId="{23F2D4E7-8956-4156-B653-43BFFD3E8868}" destId="{723000EF-22DF-4167-B710-9FF66AE068F7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{9E105874-874A-445C-BE35-A85BEE05763C}" type="presOf" srcId="{A01F4A42-1918-4A19-8090-8A089D6BD25A}" destId="{F2C593C8-199E-4BE8-A2F4-C6746DA80C23}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{63A9645E-A238-4198-9318-34BA778C5D19}" type="presOf" srcId="{1EB06E8D-2BC4-45A7-B495-A32A288B2EE2}" destId="{68258DD7-C49E-4C7F-9F88-F5D2DC20D36B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
+    <dgm:cxn modelId="{7645E34D-DABC-4807-BEB7-AF42A3C4957F}" srcId="{0CB4F66B-7CD5-4AC2-840F-428C50763456}" destId="{1EB06E8D-2BC4-45A7-B495-A32A288B2EE2}" srcOrd="0" destOrd="0" parTransId="{8034FF05-EF39-421C-8E54-F5BF7FFDB845}" sibTransId="{23F2D4E7-8956-4156-B653-43BFFD3E8868}"/>
     <dgm:cxn modelId="{4A3EAF23-CECB-4C42-9D57-84CAC297AB9E}" type="presOf" srcId="{3F994207-2612-453E-A085-A37710E7F755}" destId="{3C669D7C-9D20-4333-8B9B-7AF4764D3499}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
-    <dgm:cxn modelId="{7645E34D-DABC-4807-BEB7-AF42A3C4957F}" srcId="{0CB4F66B-7CD5-4AC2-840F-428C50763456}" destId="{1EB06E8D-2BC4-45A7-B495-A32A288B2EE2}" srcOrd="0" destOrd="0" parTransId="{8034FF05-EF39-421C-8E54-F5BF7FFDB845}" sibTransId="{23F2D4E7-8956-4156-B653-43BFFD3E8868}"/>
     <dgm:cxn modelId="{569FE7D5-FF84-4699-978B-544BD056640D}" type="presOf" srcId="{3F994207-2612-453E-A085-A37710E7F755}" destId="{F0DF1363-D6A2-49C2-A60C-3630AFB61E67}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{C8425EC8-3050-48DF-9DC2-63E8A820F2AF}" type="presOf" srcId="{D1F4FBF3-0DDB-4943-9E2C-1C88BE4D0831}" destId="{EE8F5E6F-4C60-4DAA-94DE-61E5FFCF9287}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{C75152B6-4B6C-4A4B-86C3-79D1713AC2FC}" srcId="{0CB4F66B-7CD5-4AC2-840F-428C50763456}" destId="{A01F4A42-1918-4A19-8090-8A089D6BD25A}" srcOrd="1" destOrd="0" parTransId="{9EA173EC-AFEA-488D-87E0-435A34C3E589}" sibTransId="{3F994207-2612-453E-A085-A37710E7F755}"/>
@@ -6501,10 +6712,24 @@
     <dgm:pt modelId="{9A7527AB-9941-44A3-9BD0-A227C43F6EA6}" type="pres">
       <dgm:prSet presAssocID="{CEF4CFDB-9EA8-4417-8184-BEBF0CCC7B5B}" presName="sibTrans" presStyleLbl="sibTrans2D1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{7BB59659-D4CD-4611-8DA1-E448326452C8}" type="pres">
       <dgm:prSet presAssocID="{CEF4CFDB-9EA8-4417-8184-BEBF0CCC7B5B}" presName="connectorText" presStyleLbl="sibTrans2D1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{0F0517EC-DB36-488A-BC4D-FD2F9C90D918}" type="pres">
       <dgm:prSet presAssocID="{4DE2580C-E6AC-4D86-A6D8-5C9479BA5B53}" presName="node" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="2">
@@ -6523,8 +6748,8 @@
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
+    <dgm:cxn modelId="{00DE2B24-D097-463E-AAF3-F682D4F6A848}" type="presOf" srcId="{4DE2580C-E6AC-4D86-A6D8-5C9479BA5B53}" destId="{0F0517EC-DB36-488A-BC4D-FD2F9C90D918}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{CC8E6A04-07F9-42AF-9AEA-79CD4FBCCC48}" srcId="{651C1653-D665-44FB-A133-63672E6A8C16}" destId="{4DE2580C-E6AC-4D86-A6D8-5C9479BA5B53}" srcOrd="1" destOrd="0" parTransId="{E77A4371-17AD-46DA-AF95-1A74CB896D5D}" sibTransId="{64BAD746-9F60-463A-9D7E-C921F211E5EA}"/>
-    <dgm:cxn modelId="{00DE2B24-D097-463E-AAF3-F682D4F6A848}" type="presOf" srcId="{4DE2580C-E6AC-4D86-A6D8-5C9479BA5B53}" destId="{0F0517EC-DB36-488A-BC4D-FD2F9C90D918}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{F48DC641-6071-4BD8-90CE-4A6684C7BAE1}" srcId="{651C1653-D665-44FB-A133-63672E6A8C16}" destId="{040D2348-52E0-4147-A55E-07BD2CBE5DF4}" srcOrd="0" destOrd="0" parTransId="{2F37A1A3-3D41-4B4C-89CD-14C927B09B94}" sibTransId="{CEF4CFDB-9EA8-4417-8184-BEBF0CCC7B5B}"/>
     <dgm:cxn modelId="{2B768A40-4830-493A-8005-7063A3C7DC62}" type="presOf" srcId="{651C1653-D665-44FB-A133-63672E6A8C16}" destId="{1D3B814A-FDCF-4FFF-AE42-BCC69510708B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{302243A6-8610-44EB-A6C9-D0B07942CC24}" type="presOf" srcId="{040D2348-52E0-4147-A55E-07BD2CBE5DF4}" destId="{7A7886BC-3CB6-438E-BF36-8D7E43B4D0C9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
@@ -6651,10 +6876,24 @@
     <dgm:pt modelId="{9A7527AB-9941-44A3-9BD0-A227C43F6EA6}" type="pres">
       <dgm:prSet presAssocID="{CEF4CFDB-9EA8-4417-8184-BEBF0CCC7B5B}" presName="sibTrans" presStyleLbl="sibTrans2D1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{7BB59659-D4CD-4611-8DA1-E448326452C8}" type="pres">
       <dgm:prSet presAssocID="{CEF4CFDB-9EA8-4417-8184-BEBF0CCC7B5B}" presName="connectorText" presStyleLbl="sibTrans2D1" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{0F0517EC-DB36-488A-BC4D-FD2F9C90D918}" type="pres">
       <dgm:prSet presAssocID="{4DE2580C-E6AC-4D86-A6D8-5C9479BA5B53}" presName="node" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="2">
@@ -6677,8 +6916,8 @@
     <dgm:cxn modelId="{F48DC641-6071-4BD8-90CE-4A6684C7BAE1}" srcId="{651C1653-D665-44FB-A133-63672E6A8C16}" destId="{040D2348-52E0-4147-A55E-07BD2CBE5DF4}" srcOrd="0" destOrd="0" parTransId="{2F37A1A3-3D41-4B4C-89CD-14C927B09B94}" sibTransId="{CEF4CFDB-9EA8-4417-8184-BEBF0CCC7B5B}"/>
     <dgm:cxn modelId="{ACE6CA34-8C36-4DBE-B42B-CF43DB42DD67}" type="presOf" srcId="{4DE2580C-E6AC-4D86-A6D8-5C9479BA5B53}" destId="{0F0517EC-DB36-488A-BC4D-FD2F9C90D918}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{3F0811BF-7379-44F2-9E1F-DBC965A99D9B}" type="presOf" srcId="{CEF4CFDB-9EA8-4417-8184-BEBF0CCC7B5B}" destId="{9A7527AB-9941-44A3-9BD0-A227C43F6EA6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
+    <dgm:cxn modelId="{E969C12F-7EAE-4D9A-B2DE-CE01A5749C90}" type="presOf" srcId="{CEF4CFDB-9EA8-4417-8184-BEBF0CCC7B5B}" destId="{7BB59659-D4CD-4611-8DA1-E448326452C8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{BA0E09F9-D044-4C10-94EA-3CEFA12E948F}" type="presOf" srcId="{040D2348-52E0-4147-A55E-07BD2CBE5DF4}" destId="{7A7886BC-3CB6-438E-BF36-8D7E43B4D0C9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
-    <dgm:cxn modelId="{E969C12F-7EAE-4D9A-B2DE-CE01A5749C90}" type="presOf" srcId="{CEF4CFDB-9EA8-4417-8184-BEBF0CCC7B5B}" destId="{7BB59659-D4CD-4611-8DA1-E448326452C8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{90A76FFD-8D73-4F6C-8BA6-E800904F678E}" type="presOf" srcId="{651C1653-D665-44FB-A133-63672E6A8C16}" destId="{1D3B814A-FDCF-4FFF-AE42-BCC69510708B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{A4E0E42A-D4A6-4BAA-8921-FA824155CFDF}" type="presParOf" srcId="{1D3B814A-FDCF-4FFF-AE42-BCC69510708B}" destId="{7A7886BC-3CB6-438E-BF36-8D7E43B4D0C9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
     <dgm:cxn modelId="{4BD501E2-7D14-4968-847F-BF3EDD7E9DAE}" type="presParOf" srcId="{1D3B814A-FDCF-4FFF-AE42-BCC69510708B}" destId="{9A7527AB-9941-44A3-9BD0-A227C43F6EA6}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/process1"/>
@@ -8038,7 +8277,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1300" kern="1200"/>
-            <a:t>Ready</a:t>
+            <a:t>In Progress</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
@@ -8185,7 +8424,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1300" kern="1200"/>
-            <a:t>In Progress</a:t>
+            <a:t>In Review</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
@@ -18781,126 +19020,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Rectangle 22"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10382250" y="3905250"/>
-          <a:ext cx="2076450" cy="95250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FF0000"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="Flowchart: Manual Operation 27"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6124575" y="4191000"/>
-          <a:ext cx="6086475" cy="1228725"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartManualOperation">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B050"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>57151</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -19085,15 +19204,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -19102,7 +19221,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="180974" y="4800600"/>
+          <a:off x="276224" y="4953000"/>
           <a:ext cx="3790951" cy="923925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -19294,6 +19413,447 @@
             <a:t> With Stage Gates</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="4000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>390526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Freeform 43"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6076950" y="4124326"/>
+          <a:ext cx="5924550" cy="1219200"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 57150 w 2924175"/>
+            <a:gd name="connsiteY0" fmla="*/ 733425 h 847725"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2924175"/>
+            <a:gd name="connsiteY1" fmla="*/ 657225 h 847725"/>
+            <a:gd name="connsiteX2" fmla="*/ 800100 w 2924175"/>
+            <a:gd name="connsiteY2" fmla="*/ 542925 h 847725"/>
+            <a:gd name="connsiteX3" fmla="*/ 1085850 w 2924175"/>
+            <a:gd name="connsiteY3" fmla="*/ 333375 h 847725"/>
+            <a:gd name="connsiteX4" fmla="*/ 1362075 w 2924175"/>
+            <a:gd name="connsiteY4" fmla="*/ 171450 h 847725"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2924175"/>
+            <a:gd name="connsiteY5" fmla="*/ 57150 h 847725"/>
+            <a:gd name="connsiteX6" fmla="*/ 2247900 w 2924175"/>
+            <a:gd name="connsiteY6" fmla="*/ 0 h 847725"/>
+            <a:gd name="connsiteX7" fmla="*/ 2924175 w 2924175"/>
+            <a:gd name="connsiteY7" fmla="*/ 0 h 847725"/>
+            <a:gd name="connsiteX8" fmla="*/ 2914650 w 2924175"/>
+            <a:gd name="connsiteY8" fmla="*/ 809625 h 847725"/>
+            <a:gd name="connsiteX9" fmla="*/ 0 w 2924175"/>
+            <a:gd name="connsiteY9" fmla="*/ 847725 h 847725"/>
+            <a:gd name="connsiteX10" fmla="*/ 57150 w 2924175"/>
+            <a:gd name="connsiteY10" fmla="*/ 733425 h 847725"/>
+            <a:gd name="connsiteX0" fmla="*/ 57150 w 2924175"/>
+            <a:gd name="connsiteY0" fmla="*/ 733425 h 847725"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2924175"/>
+            <a:gd name="connsiteY1" fmla="*/ 657225 h 847725"/>
+            <a:gd name="connsiteX2" fmla="*/ 800100 w 2924175"/>
+            <a:gd name="connsiteY2" fmla="*/ 542925 h 847725"/>
+            <a:gd name="connsiteX3" fmla="*/ 1085850 w 2924175"/>
+            <a:gd name="connsiteY3" fmla="*/ 333375 h 847725"/>
+            <a:gd name="connsiteX4" fmla="*/ 1362075 w 2924175"/>
+            <a:gd name="connsiteY4" fmla="*/ 171450 h 847725"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2924175"/>
+            <a:gd name="connsiteY5" fmla="*/ 57150 h 847725"/>
+            <a:gd name="connsiteX6" fmla="*/ 2247900 w 2924175"/>
+            <a:gd name="connsiteY6" fmla="*/ 0 h 847725"/>
+            <a:gd name="connsiteX7" fmla="*/ 2924175 w 2924175"/>
+            <a:gd name="connsiteY7" fmla="*/ 0 h 847725"/>
+            <a:gd name="connsiteX8" fmla="*/ 2920534 w 2924175"/>
+            <a:gd name="connsiteY8" fmla="*/ 833173 h 847725"/>
+            <a:gd name="connsiteX9" fmla="*/ 0 w 2924175"/>
+            <a:gd name="connsiteY9" fmla="*/ 847725 h 847725"/>
+            <a:gd name="connsiteX10" fmla="*/ 57150 w 2924175"/>
+            <a:gd name="connsiteY10" fmla="*/ 733425 h 847725"/>
+            <a:gd name="connsiteX0" fmla="*/ 186591 w 2924175"/>
+            <a:gd name="connsiteY0" fmla="*/ 780521 h 847725"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2924175"/>
+            <a:gd name="connsiteY1" fmla="*/ 657225 h 847725"/>
+            <a:gd name="connsiteX2" fmla="*/ 800100 w 2924175"/>
+            <a:gd name="connsiteY2" fmla="*/ 542925 h 847725"/>
+            <a:gd name="connsiteX3" fmla="*/ 1085850 w 2924175"/>
+            <a:gd name="connsiteY3" fmla="*/ 333375 h 847725"/>
+            <a:gd name="connsiteX4" fmla="*/ 1362075 w 2924175"/>
+            <a:gd name="connsiteY4" fmla="*/ 171450 h 847725"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2924175"/>
+            <a:gd name="connsiteY5" fmla="*/ 57150 h 847725"/>
+            <a:gd name="connsiteX6" fmla="*/ 2247900 w 2924175"/>
+            <a:gd name="connsiteY6" fmla="*/ 0 h 847725"/>
+            <a:gd name="connsiteX7" fmla="*/ 2924175 w 2924175"/>
+            <a:gd name="connsiteY7" fmla="*/ 0 h 847725"/>
+            <a:gd name="connsiteX8" fmla="*/ 2920534 w 2924175"/>
+            <a:gd name="connsiteY8" fmla="*/ 833173 h 847725"/>
+            <a:gd name="connsiteX9" fmla="*/ 0 w 2924175"/>
+            <a:gd name="connsiteY9" fmla="*/ 847725 h 847725"/>
+            <a:gd name="connsiteX10" fmla="*/ 186591 w 2924175"/>
+            <a:gd name="connsiteY10" fmla="*/ 780521 h 847725"/>
+            <a:gd name="connsiteX0" fmla="*/ 227777 w 2924175"/>
+            <a:gd name="connsiteY0" fmla="*/ 788370 h 847725"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2924175"/>
+            <a:gd name="connsiteY1" fmla="*/ 657225 h 847725"/>
+            <a:gd name="connsiteX2" fmla="*/ 800100 w 2924175"/>
+            <a:gd name="connsiteY2" fmla="*/ 542925 h 847725"/>
+            <a:gd name="connsiteX3" fmla="*/ 1085850 w 2924175"/>
+            <a:gd name="connsiteY3" fmla="*/ 333375 h 847725"/>
+            <a:gd name="connsiteX4" fmla="*/ 1362075 w 2924175"/>
+            <a:gd name="connsiteY4" fmla="*/ 171450 h 847725"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2924175"/>
+            <a:gd name="connsiteY5" fmla="*/ 57150 h 847725"/>
+            <a:gd name="connsiteX6" fmla="*/ 2247900 w 2924175"/>
+            <a:gd name="connsiteY6" fmla="*/ 0 h 847725"/>
+            <a:gd name="connsiteX7" fmla="*/ 2924175 w 2924175"/>
+            <a:gd name="connsiteY7" fmla="*/ 0 h 847725"/>
+            <a:gd name="connsiteX8" fmla="*/ 2920534 w 2924175"/>
+            <a:gd name="connsiteY8" fmla="*/ 833173 h 847725"/>
+            <a:gd name="connsiteX9" fmla="*/ 0 w 2924175"/>
+            <a:gd name="connsiteY9" fmla="*/ 847725 h 847725"/>
+            <a:gd name="connsiteX10" fmla="*/ 227777 w 2924175"/>
+            <a:gd name="connsiteY10" fmla="*/ 788370 h 847725"/>
+            <a:gd name="connsiteX0" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY0" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2930059"/>
+            <a:gd name="connsiteY1" fmla="*/ 727869 h 918369"/>
+            <a:gd name="connsiteX2" fmla="*/ 800100 w 2930059"/>
+            <a:gd name="connsiteY2" fmla="*/ 613569 h 918369"/>
+            <a:gd name="connsiteX3" fmla="*/ 1085850 w 2930059"/>
+            <a:gd name="connsiteY3" fmla="*/ 404019 h 918369"/>
+            <a:gd name="connsiteX4" fmla="*/ 1362075 w 2930059"/>
+            <a:gd name="connsiteY4" fmla="*/ 242094 h 918369"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2930059"/>
+            <a:gd name="connsiteY5" fmla="*/ 127794 h 918369"/>
+            <a:gd name="connsiteX6" fmla="*/ 2247900 w 2930059"/>
+            <a:gd name="connsiteY6" fmla="*/ 70644 h 918369"/>
+            <a:gd name="connsiteX7" fmla="*/ 2930059 w 2930059"/>
+            <a:gd name="connsiteY7" fmla="*/ 0 h 918369"/>
+            <a:gd name="connsiteX8" fmla="*/ 2920534 w 2930059"/>
+            <a:gd name="connsiteY8" fmla="*/ 903817 h 918369"/>
+            <a:gd name="connsiteX9" fmla="*/ 0 w 2930059"/>
+            <a:gd name="connsiteY9" fmla="*/ 918369 h 918369"/>
+            <a:gd name="connsiteX10" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY10" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX0" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY0" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2930059"/>
+            <a:gd name="connsiteY1" fmla="*/ 727869 h 918369"/>
+            <a:gd name="connsiteX2" fmla="*/ 800100 w 2930059"/>
+            <a:gd name="connsiteY2" fmla="*/ 613569 h 918369"/>
+            <a:gd name="connsiteX3" fmla="*/ 1085850 w 2930059"/>
+            <a:gd name="connsiteY3" fmla="*/ 404019 h 918369"/>
+            <a:gd name="connsiteX4" fmla="*/ 1362075 w 2930059"/>
+            <a:gd name="connsiteY4" fmla="*/ 242094 h 918369"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2930059"/>
+            <a:gd name="connsiteY5" fmla="*/ 127794 h 918369"/>
+            <a:gd name="connsiteX6" fmla="*/ 2247900 w 2930059"/>
+            <a:gd name="connsiteY6" fmla="*/ 70644 h 918369"/>
+            <a:gd name="connsiteX7" fmla="*/ 2657371 w 2930059"/>
+            <a:gd name="connsiteY7" fmla="*/ 31397 h 918369"/>
+            <a:gd name="connsiteX8" fmla="*/ 2930059 w 2930059"/>
+            <a:gd name="connsiteY8" fmla="*/ 0 h 918369"/>
+            <a:gd name="connsiteX9" fmla="*/ 2920534 w 2930059"/>
+            <a:gd name="connsiteY9" fmla="*/ 903817 h 918369"/>
+            <a:gd name="connsiteX10" fmla="*/ 0 w 2930059"/>
+            <a:gd name="connsiteY10" fmla="*/ 918369 h 918369"/>
+            <a:gd name="connsiteX11" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY11" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX0" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY0" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2930059"/>
+            <a:gd name="connsiteY1" fmla="*/ 727869 h 918369"/>
+            <a:gd name="connsiteX2" fmla="*/ 800100 w 2930059"/>
+            <a:gd name="connsiteY2" fmla="*/ 613569 h 918369"/>
+            <a:gd name="connsiteX3" fmla="*/ 1085850 w 2930059"/>
+            <a:gd name="connsiteY3" fmla="*/ 404019 h 918369"/>
+            <a:gd name="connsiteX4" fmla="*/ 1362075 w 2930059"/>
+            <a:gd name="connsiteY4" fmla="*/ 242094 h 918369"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2930059"/>
+            <a:gd name="connsiteY5" fmla="*/ 127794 h 918369"/>
+            <a:gd name="connsiteX6" fmla="*/ 2247900 w 2930059"/>
+            <a:gd name="connsiteY6" fmla="*/ 70644 h 918369"/>
+            <a:gd name="connsiteX7" fmla="*/ 2657371 w 2930059"/>
+            <a:gd name="connsiteY7" fmla="*/ 0 h 918369"/>
+            <a:gd name="connsiteX8" fmla="*/ 2930059 w 2930059"/>
+            <a:gd name="connsiteY8" fmla="*/ 0 h 918369"/>
+            <a:gd name="connsiteX9" fmla="*/ 2920534 w 2930059"/>
+            <a:gd name="connsiteY9" fmla="*/ 903817 h 918369"/>
+            <a:gd name="connsiteX10" fmla="*/ 0 w 2930059"/>
+            <a:gd name="connsiteY10" fmla="*/ 918369 h 918369"/>
+            <a:gd name="connsiteX11" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY11" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX0" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY0" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2930059"/>
+            <a:gd name="connsiteY1" fmla="*/ 727869 h 918369"/>
+            <a:gd name="connsiteX2" fmla="*/ 800100 w 2930059"/>
+            <a:gd name="connsiteY2" fmla="*/ 613569 h 918369"/>
+            <a:gd name="connsiteX3" fmla="*/ 1085850 w 2930059"/>
+            <a:gd name="connsiteY3" fmla="*/ 404019 h 918369"/>
+            <a:gd name="connsiteX4" fmla="*/ 1362075 w 2930059"/>
+            <a:gd name="connsiteY4" fmla="*/ 242094 h 918369"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2930059"/>
+            <a:gd name="connsiteY5" fmla="*/ 127794 h 918369"/>
+            <a:gd name="connsiteX6" fmla="*/ 2247900 w 2930059"/>
+            <a:gd name="connsiteY6" fmla="*/ 70644 h 918369"/>
+            <a:gd name="connsiteX7" fmla="*/ 2765717 w 2930059"/>
+            <a:gd name="connsiteY7" fmla="*/ 7175 h 918369"/>
+            <a:gd name="connsiteX8" fmla="*/ 2930059 w 2930059"/>
+            <a:gd name="connsiteY8" fmla="*/ 0 h 918369"/>
+            <a:gd name="connsiteX9" fmla="*/ 2920534 w 2930059"/>
+            <a:gd name="connsiteY9" fmla="*/ 903817 h 918369"/>
+            <a:gd name="connsiteX10" fmla="*/ 0 w 2930059"/>
+            <a:gd name="connsiteY10" fmla="*/ 918369 h 918369"/>
+            <a:gd name="connsiteX11" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY11" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX0" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY0" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2930059"/>
+            <a:gd name="connsiteY1" fmla="*/ 727869 h 918369"/>
+            <a:gd name="connsiteX2" fmla="*/ 800100 w 2930059"/>
+            <a:gd name="connsiteY2" fmla="*/ 613569 h 918369"/>
+            <a:gd name="connsiteX3" fmla="*/ 1085850 w 2930059"/>
+            <a:gd name="connsiteY3" fmla="*/ 404019 h 918369"/>
+            <a:gd name="connsiteX4" fmla="*/ 1362075 w 2930059"/>
+            <a:gd name="connsiteY4" fmla="*/ 242094 h 918369"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2930059"/>
+            <a:gd name="connsiteY5" fmla="*/ 127794 h 918369"/>
+            <a:gd name="connsiteX6" fmla="*/ 2295007 w 2930059"/>
+            <a:gd name="connsiteY6" fmla="*/ 49120 h 918369"/>
+            <a:gd name="connsiteX7" fmla="*/ 2765717 w 2930059"/>
+            <a:gd name="connsiteY7" fmla="*/ 7175 h 918369"/>
+            <a:gd name="connsiteX8" fmla="*/ 2930059 w 2930059"/>
+            <a:gd name="connsiteY8" fmla="*/ 0 h 918369"/>
+            <a:gd name="connsiteX9" fmla="*/ 2920534 w 2930059"/>
+            <a:gd name="connsiteY9" fmla="*/ 903817 h 918369"/>
+            <a:gd name="connsiteX10" fmla="*/ 0 w 2930059"/>
+            <a:gd name="connsiteY10" fmla="*/ 918369 h 918369"/>
+            <a:gd name="connsiteX11" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY11" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX0" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY0" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2930059"/>
+            <a:gd name="connsiteY1" fmla="*/ 727869 h 918369"/>
+            <a:gd name="connsiteX2" fmla="*/ 800100 w 2930059"/>
+            <a:gd name="connsiteY2" fmla="*/ 613569 h 918369"/>
+            <a:gd name="connsiteX3" fmla="*/ 1085850 w 2930059"/>
+            <a:gd name="connsiteY3" fmla="*/ 404019 h 918369"/>
+            <a:gd name="connsiteX4" fmla="*/ 1489264 w 2930059"/>
+            <a:gd name="connsiteY4" fmla="*/ 263618 h 918369"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2930059"/>
+            <a:gd name="connsiteY5" fmla="*/ 127794 h 918369"/>
+            <a:gd name="connsiteX6" fmla="*/ 2295007 w 2930059"/>
+            <a:gd name="connsiteY6" fmla="*/ 49120 h 918369"/>
+            <a:gd name="connsiteX7" fmla="*/ 2765717 w 2930059"/>
+            <a:gd name="connsiteY7" fmla="*/ 7175 h 918369"/>
+            <a:gd name="connsiteX8" fmla="*/ 2930059 w 2930059"/>
+            <a:gd name="connsiteY8" fmla="*/ 0 h 918369"/>
+            <a:gd name="connsiteX9" fmla="*/ 2920534 w 2930059"/>
+            <a:gd name="connsiteY9" fmla="*/ 903817 h 918369"/>
+            <a:gd name="connsiteX10" fmla="*/ 0 w 2930059"/>
+            <a:gd name="connsiteY10" fmla="*/ 918369 h 918369"/>
+            <a:gd name="connsiteX11" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY11" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX0" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY0" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2930059"/>
+            <a:gd name="connsiteY1" fmla="*/ 727869 h 918369"/>
+            <a:gd name="connsiteX2" fmla="*/ 800100 w 2930059"/>
+            <a:gd name="connsiteY2" fmla="*/ 613569 h 918369"/>
+            <a:gd name="connsiteX3" fmla="*/ 1081139 w 2930059"/>
+            <a:gd name="connsiteY3" fmla="*/ 518815 h 918369"/>
+            <a:gd name="connsiteX4" fmla="*/ 1489264 w 2930059"/>
+            <a:gd name="connsiteY4" fmla="*/ 263618 h 918369"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2930059"/>
+            <a:gd name="connsiteY5" fmla="*/ 127794 h 918369"/>
+            <a:gd name="connsiteX6" fmla="*/ 2295007 w 2930059"/>
+            <a:gd name="connsiteY6" fmla="*/ 49120 h 918369"/>
+            <a:gd name="connsiteX7" fmla="*/ 2765717 w 2930059"/>
+            <a:gd name="connsiteY7" fmla="*/ 7175 h 918369"/>
+            <a:gd name="connsiteX8" fmla="*/ 2930059 w 2930059"/>
+            <a:gd name="connsiteY8" fmla="*/ 0 h 918369"/>
+            <a:gd name="connsiteX9" fmla="*/ 2920534 w 2930059"/>
+            <a:gd name="connsiteY9" fmla="*/ 903817 h 918369"/>
+            <a:gd name="connsiteX10" fmla="*/ 0 w 2930059"/>
+            <a:gd name="connsiteY10" fmla="*/ 918369 h 918369"/>
+            <a:gd name="connsiteX11" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY11" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX0" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY0" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX1" fmla="*/ 504825 w 2930059"/>
+            <a:gd name="connsiteY1" fmla="*/ 727869 h 918369"/>
+            <a:gd name="connsiteX2" fmla="*/ 804811 w 2930059"/>
+            <a:gd name="connsiteY2" fmla="*/ 678142 h 918369"/>
+            <a:gd name="connsiteX3" fmla="*/ 1081139 w 2930059"/>
+            <a:gd name="connsiteY3" fmla="*/ 518815 h 918369"/>
+            <a:gd name="connsiteX4" fmla="*/ 1489264 w 2930059"/>
+            <a:gd name="connsiteY4" fmla="*/ 263618 h 918369"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2930059"/>
+            <a:gd name="connsiteY5" fmla="*/ 127794 h 918369"/>
+            <a:gd name="connsiteX6" fmla="*/ 2295007 w 2930059"/>
+            <a:gd name="connsiteY6" fmla="*/ 49120 h 918369"/>
+            <a:gd name="connsiteX7" fmla="*/ 2765717 w 2930059"/>
+            <a:gd name="connsiteY7" fmla="*/ 7175 h 918369"/>
+            <a:gd name="connsiteX8" fmla="*/ 2930059 w 2930059"/>
+            <a:gd name="connsiteY8" fmla="*/ 0 h 918369"/>
+            <a:gd name="connsiteX9" fmla="*/ 2920534 w 2930059"/>
+            <a:gd name="connsiteY9" fmla="*/ 903817 h 918369"/>
+            <a:gd name="connsiteX10" fmla="*/ 0 w 2930059"/>
+            <a:gd name="connsiteY10" fmla="*/ 918369 h 918369"/>
+            <a:gd name="connsiteX11" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY11" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX0" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY0" fmla="*/ 859014 h 918369"/>
+            <a:gd name="connsiteX1" fmla="*/ 500114 w 2930059"/>
+            <a:gd name="connsiteY1" fmla="*/ 778093 h 918369"/>
+            <a:gd name="connsiteX2" fmla="*/ 804811 w 2930059"/>
+            <a:gd name="connsiteY2" fmla="*/ 678142 h 918369"/>
+            <a:gd name="connsiteX3" fmla="*/ 1081139 w 2930059"/>
+            <a:gd name="connsiteY3" fmla="*/ 518815 h 918369"/>
+            <a:gd name="connsiteX4" fmla="*/ 1489264 w 2930059"/>
+            <a:gd name="connsiteY4" fmla="*/ 263618 h 918369"/>
+            <a:gd name="connsiteX5" fmla="*/ 1819275 w 2930059"/>
+            <a:gd name="connsiteY5" fmla="*/ 127794 h 918369"/>
+            <a:gd name="connsiteX6" fmla="*/ 2295007 w 2930059"/>
+            <a:gd name="connsiteY6" fmla="*/ 49120 h 918369"/>
+            <a:gd name="connsiteX7" fmla="*/ 2765717 w 2930059"/>
+            <a:gd name="connsiteY7" fmla="*/ 7175 h 918369"/>
+            <a:gd name="connsiteX8" fmla="*/ 2930059 w 2930059"/>
+            <a:gd name="connsiteY8" fmla="*/ 0 h 918369"/>
+            <a:gd name="connsiteX9" fmla="*/ 2920534 w 2930059"/>
+            <a:gd name="connsiteY9" fmla="*/ 903817 h 918369"/>
+            <a:gd name="connsiteX10" fmla="*/ 0 w 2930059"/>
+            <a:gd name="connsiteY10" fmla="*/ 918369 h 918369"/>
+            <a:gd name="connsiteX11" fmla="*/ 227777 w 2930059"/>
+            <a:gd name="connsiteY11" fmla="*/ 859014 h 918369"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2930059" h="918369">
+              <a:moveTo>
+                <a:pt x="227777" y="859014"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="500114" y="778093"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="804811" y="678142"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1081139" y="518815"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1489264" y="263618"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1819275" y="127794"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2295007" y="49120"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2765717" y="7175"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2930059" y="0"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="2928845" y="277724"/>
+                <a:pt x="2921748" y="626093"/>
+                <a:pt x="2920534" y="903817"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="0" y="918369"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="227777" y="859014"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -20608,7 +21168,7 @@
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:rPr>
-              <a:t> new customer </a:t>
+              <a:t> user, </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
@@ -20619,29 +21179,7 @@
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:rPr>
-              <a:t>I want </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100" b="1" i="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t>a web interface </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t>so  I can use it on my PC</a:t>
+              <a:t>I want to control who can see my posts so that my information is secure</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB" sz="1100" b="1" i="0">
               <a:solidFill>
@@ -20712,7 +21250,7 @@
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:rPr>
-              <a:t> new customer </a:t>
+              <a:t> user </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
@@ -20734,7 +21272,7 @@
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:rPr>
-              <a:t>download the app</a:t>
+              <a:t>change my password </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
@@ -20745,7 +21283,7 @@
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:rPr>
-              <a:t> so that I </a:t>
+              <a:t>so that </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" sz="1100" b="1" i="0" baseline="0">
@@ -20756,7 +21294,7 @@
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:rPr>
-              <a:t>can use it on my phone</a:t>
+              <a:t>my account is secure</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB" sz="1100" b="1" i="0">
               <a:solidFill>
@@ -22297,6 +22835,1841 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="90" name="Rectangle 89"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="57150" y="142875"/>
+          <a:ext cx="16878300" cy="6581775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3933826" y="523875"/>
+          <a:ext cx="3133724" cy="1152525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1"/>
+            <a:t>Agile</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1" baseline="0"/>
+            <a:t> Management Tool </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>eg.  JIRA, zube.io</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>- used for: backlog management, progress monitoring</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3905250" y="2390775"/>
+          <a:ext cx="3133724" cy="1495425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1"/>
+            <a:t>Source</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1" baseline="0"/>
+            <a:t> Control </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1"/>
+            <a:t>GitHub</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1800" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>- used for:  source code management, revision control in relation to agile workflow, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>- also potentially documentation management</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7953375" y="2324099"/>
+          <a:ext cx="3133724" cy="1800225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1800" b="1"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1"/>
+            <a:t>Continual Integration </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1" baseline="0"/>
+            <a:t>Test Tools</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" baseline="0"/>
+            <a:t>eg. Jenkins, BuddyBuild, Fitnesse...</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1200" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>- used for: automatic compilation and testing of code, notification of failures, logging of results.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8077200" y="552450"/>
+          <a:ext cx="3133724" cy="1152525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1"/>
+            <a:t>Release </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1" baseline="0"/>
+            <a:t>Tools </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>eg. FastLane, Installer projects</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>- used for  releasing code into market </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3838575" y="4991100"/>
+          <a:ext cx="3133724" cy="1314450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1800" b="1"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1"/>
+            <a:t>Developer Tools</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1800" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>- used for:  code development , testing, documentation, etc</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Down Arrow 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4067175" y="3829050"/>
+          <a:ext cx="819150" cy="1228725"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Down Arrow 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5715000" y="3819524"/>
+          <a:ext cx="819150" cy="1247775"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Down Arrow 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5038725" y="1485900"/>
+          <a:ext cx="819150" cy="904875"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="TextBox 20"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11811000" y="552450"/>
+          <a:ext cx="3133724" cy="1152525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1" baseline="0"/>
+            <a:t>Deployed Products </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>eg. AppStore</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>Azure </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>- accessed by customers to obtain value delivered</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>233363</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Down Arrow 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="7046119" y="2583657"/>
+          <a:ext cx="819150" cy="1033462"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Down Arrow 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9096375" y="1419226"/>
+          <a:ext cx="819150" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>576263</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Down Arrow 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="11060907" y="511969"/>
+          <a:ext cx="819150" cy="1062037"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>488496</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>15744</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>242222</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 4" descr="C:\Users\Jamies\AppData\Local\Microsoft\Windows\INetCache\IE\2D8HPRO6\people-man-blue-shirt[1].png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1707696" y="777744"/>
+          <a:ext cx="972926" cy="860556"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>8622</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rectangle 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="981075" y="323850"/>
+          <a:ext cx="2352675" cy="827772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Product</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Owner</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352986</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 5" descr="C:\Users\Jamies\AppData\Local\Microsoft\Windows\INetCache\IE\12BHOXPN\Emblem-person-red.svg[1].png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1562100" y="2276475"/>
+          <a:ext cx="1229286" cy="1238250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>65772</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Rectangle 31"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="1905000"/>
+          <a:ext cx="2352675" cy="827772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Scrum Master</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114859</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="33" name="Group 32"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="885826" y="4429125"/>
+          <a:ext cx="1828800" cy="1400734"/>
+          <a:chOff x="9917205" y="4812801"/>
+          <a:chExt cx="2187387" cy="1507316"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="34" name="Picture 6" descr="C:\Users\Jamies\AppData\Local\Microsoft\Windows\INetCache\IE\971OSSCB\1024px-Emblem-person-orange.svg[1].png"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="10726269" y="4815043"/>
+            <a:ext cx="1378323" cy="1388533"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="35" name="Picture 6" descr="C:\Users\Jamies\AppData\Local\Microsoft\Windows\INetCache\IE\971OSSCB\1024px-Emblem-person-orange.svg[1].png"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="9917205" y="4812801"/>
+            <a:ext cx="1378323" cy="1388533"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="36" name="Picture 6" descr="C:\Users\Jamies\AppData\Local\Microsoft\Windows\INetCache\IE\971OSSCB\1024px-Emblem-person-orange.svg[1].png"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="10282516" y="4931584"/>
+            <a:ext cx="1378323" cy="1388533"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>94347</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="Rectangle 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628650" y="4029075"/>
+          <a:ext cx="2352675" cy="827772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Team Members</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Straight Arrow Connector 63"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2809875" y="1085850"/>
+          <a:ext cx="1038225" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="65" name="Straight Arrow Connector 64"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2790825" y="1600201"/>
+          <a:ext cx="1028700" cy="628649"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="Straight Arrow Connector 67"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2600325" y="1800226"/>
+          <a:ext cx="1352550" cy="2457449"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Straight Arrow Connector 72"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2743200" y="2857500"/>
+          <a:ext cx="1085850" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="74" name="Straight Arrow Connector 73"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2714625" y="5276850"/>
+          <a:ext cx="1114425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Straight Arrow Connector 79"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2619375" y="3971926"/>
+          <a:ext cx="1276350" cy="723899"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>302601</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2052" name="Picture 4" descr="C:\Users\Jamies\AppData\Local\Microsoft\Windows\INetCache\IE\EIHXE8IP\5[1].jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11885001" y="2647950"/>
+          <a:ext cx="3288323" cy="1943100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>75297</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="88" name="Rectangle 87"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12620625" y="4010025"/>
+          <a:ext cx="2352675" cy="827772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Happy Customers!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="91" name="TextBox 90"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8248650" y="5715000"/>
+          <a:ext cx="7715250" cy="1009650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400" baseline="0"/>
+            <a:t>An Agile Development Environment</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="92" name="Down Arrow 91"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13011150" y="1647825"/>
+          <a:ext cx="819150" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -22584,8 +24957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C27:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X28" sqref="X28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22607,7 +24980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -22620,13 +24993,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="O33:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="33" spans="15:15" ht="23.25">
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="15:15" ht="23.25">
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="15:15">
+      <c r="O35" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>